<commit_message>
update of statistics datafile + adding new slurry TAN analysis
</commit_message>
<xml_diff>
--- a/data/slurry_soil.xlsx
+++ b/data/slurry_soil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Dokumenter/GitHub/Pedersen-2023-DFC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{40C3143B-5A87-4D22-BF96-876948DD87EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C30A201-D7BF-4307-BE1C-3F0CAA848F53}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{40C3143B-5A87-4D22-BF96-876948DD87EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{441CD53B-2E6E-48B4-B10C-25109EA9FE2E}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3045" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{A5CF0569-E470-46DA-A474-3E189588F618}"/>
+    <workbookView xWindow="-25785" yWindow="-345" windowWidth="17925" windowHeight="16110" xr2:uid="{A5CF0569-E470-46DA-A474-3E189588F618}"/>
   </bookViews>
   <sheets>
     <sheet name="slurry" sheetId="1" r:id="rId1"/>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D306BF-A2EF-4B07-A320-89D1CB5BCBE6}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,8 +525,8 @@
       <c r="F2">
         <v>2.9010000000000002</v>
       </c>
-      <c r="G2">
-        <v>1.5330000000000001</v>
+      <c r="G2" s="3">
+        <v>2.008686210640608</v>
       </c>
       <c r="H2" s="4">
         <v>7.53</v>
@@ -551,8 +551,8 @@
       <c r="F3">
         <v>2.331</v>
       </c>
-      <c r="G3">
-        <v>1.109</v>
+      <c r="G3" s="3">
+        <v>1.9821605550049555</v>
       </c>
       <c r="H3" s="4">
         <v>7.51</v>
@@ -577,8 +577,8 @@
       <c r="F4">
         <v>2.617</v>
       </c>
-      <c r="G4">
-        <v>1.516</v>
+      <c r="G4" s="3">
+        <v>1.8901890189018902</v>
       </c>
       <c r="H4" s="4">
         <v>7.51</v>
@@ -603,8 +603,8 @@
       <c r="F5">
         <v>2.597</v>
       </c>
-      <c r="G5">
-        <v>1.3240000000000001</v>
+      <c r="G5" s="3">
+        <v>1.7690875232774672</v>
       </c>
       <c r="H5" s="4">
         <v>7.49</v>
@@ -629,8 +629,8 @@
       <c r="F6">
         <v>2.6230000000000002</v>
       </c>
-      <c r="G6">
-        <v>1.2370000000000001</v>
+      <c r="G6" s="3">
+        <v>1.875</v>
       </c>
       <c r="H6" s="4">
         <v>7.58</v>
@@ -655,8 +655,8 @@
       <c r="F7">
         <v>2.8279999999999998</v>
       </c>
-      <c r="G7">
-        <v>1.4279999999999999</v>
+      <c r="G7" s="3">
+        <v>1.9762845849802373</v>
       </c>
       <c r="H7" s="4">
         <v>7.57</v>
@@ -869,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E356275-FF90-45BA-A7D6-41EFB2C7BCE3}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update app.rate for exp A DFC
</commit_message>
<xml_diff>
--- a/data/slurry_soil.xlsx
+++ b/data/slurry_soil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Dokumenter/GitHub/Pedersen-2023-DFC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{40C3143B-5A87-4D22-BF96-876948DD87EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E9FE49F-5045-4C0B-A46E-FD0392FB9045}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{40C3143B-5A87-4D22-BF96-876948DD87EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36A37698-492B-4686-B26E-B41FA67616D4}"/>
   <bookViews>
-    <workbookView xWindow="-30900" yWindow="-1290" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{A5CF0569-E470-46DA-A474-3E189588F618}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{A5CF0569-E470-46DA-A474-3E189588F618}"/>
   </bookViews>
   <sheets>
     <sheet name="slurry" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -151,7 +151,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D306BF-A2EF-4B07-A320-89D1CB5BCBE6}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -539,7 +539,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E356275-FF90-45BA-A7D6-41EFB2C7BCE3}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>